<commit_message>
Daily attendance processing - 2026-02-08 10:33:01 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7">
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -957,7 +957,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>84.2%</t>
+          <t>84.5%</t>
         </is>
       </c>
     </row>
@@ -1607,22 +1607,22 @@
         <v>54</v>
       </c>
       <c r="O19" s="5" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P19" s="5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q19" s="5" t="n">
         <v>4</v>
       </c>
       <c r="R19" s="5" t="inlineStr">
         <is>
-          <t>81.5%</t>
+          <t>83.3%</t>
         </is>
       </c>
       <c r="S19" s="5" t="inlineStr">
         <is>
-          <t>71.4%</t>
+          <t>71.5%</t>
         </is>
       </c>
     </row>
@@ -10597,45 +10597,45 @@
       </c>
     </row>
     <row r="227">
-      <c r="A227" s="4" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B227" s="4" t="inlineStr">
+      <c r="A227" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B227" s="2" t="inlineStr">
         <is>
           <t>B2E</t>
         </is>
       </c>
-      <c r="C227" s="4" t="inlineStr">
+      <c r="C227" s="2" t="inlineStr">
         <is>
           <t>CHEST</t>
         </is>
       </c>
-      <c r="D227" s="4" t="inlineStr">
+      <c r="D227" s="2" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="E227" s="4" t="inlineStr">
+      <c r="E227" s="2" t="inlineStr">
         <is>
           <t>08/02/2026</t>
         </is>
       </c>
-      <c r="F227" s="4" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G227" s="4" t="inlineStr"/>
-      <c r="H227" s="4" t="inlineStr">
-        <is>
-          <t>0/60</t>
-        </is>
-      </c>
-      <c r="I227" s="4" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F227" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G227" s="2" t="inlineStr"/>
+      <c r="H227" s="2" t="inlineStr">
+        <is>
+          <t>45/60</t>
+        </is>
+      </c>
+      <c r="I227" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-08 11:29:28 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7">
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
@@ -957,7 +957,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>84.5%</t>
+          <t>84.9%</t>
         </is>
       </c>
     </row>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>76.6%</t>
+          <t>76.3%</t>
         </is>
       </c>
     </row>
@@ -1451,22 +1451,22 @@
         <v>53</v>
       </c>
       <c r="O17" s="5" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P17" s="5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q17" s="5" t="n">
         <v>7</v>
       </c>
       <c r="R17" s="5" t="inlineStr">
         <is>
-          <t>75.5%</t>
+          <t>77.4%</t>
         </is>
       </c>
       <c r="S17" s="5" t="inlineStr">
         <is>
-          <t>80.7%</t>
+          <t>79.2%</t>
         </is>
       </c>
     </row>
@@ -6938,45 +6938,45 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="4" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B142" s="4" t="inlineStr">
+      <c r="A142" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B142" s="2" t="inlineStr">
         <is>
           <t>B2C</t>
         </is>
       </c>
-      <c r="C142" s="4" t="inlineStr">
+      <c r="C142" s="2" t="inlineStr">
         <is>
           <t>IMMUNOLOGY/HAEMATOLOGY</t>
         </is>
       </c>
-      <c r="D142" s="4" t="inlineStr">
+      <c r="D142" s="2" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="E142" s="4" t="inlineStr">
+      <c r="E142" s="2" t="inlineStr">
         <is>
           <t>08/02/2026</t>
         </is>
       </c>
-      <c r="F142" s="4" t="inlineStr">
+      <c r="F142" s="2" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G142" s="4" t="inlineStr"/>
-      <c r="H142" s="4" t="inlineStr">
-        <is>
-          <t>0/64</t>
-        </is>
-      </c>
-      <c r="I142" s="4" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="G142" s="2" t="inlineStr"/>
+      <c r="H142" s="2" t="inlineStr">
+        <is>
+          <t>13/64</t>
+        </is>
+      </c>
+      <c r="I142" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-08 11:55:10 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7">
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
@@ -957,7 +957,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>84.9%</t>
+          <t>85.3%</t>
         </is>
       </c>
     </row>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>76.3%</t>
+          <t>76.2%</t>
         </is>
       </c>
     </row>
@@ -1295,22 +1295,22 @@
         <v>53</v>
       </c>
       <c r="O15" s="5" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P15" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q15" s="5" t="n">
         <v>4</v>
       </c>
       <c r="R15" s="5" t="inlineStr">
         <is>
-          <t>83.0%</t>
+          <t>84.9%</t>
         </is>
       </c>
       <c r="S15" s="5" t="inlineStr">
         <is>
-          <t>76.5%</t>
+          <t>76.0%</t>
         </is>
       </c>
     </row>
@@ -2982,45 +2982,45 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="4" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B50" s="4" t="inlineStr">
+      <c r="A50" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="inlineStr">
         <is>
           <t>B2A</t>
         </is>
       </c>
-      <c r="C50" s="4" t="inlineStr">
+      <c r="C50" s="2" t="inlineStr">
         <is>
           <t>TROPICAL MEDICINE</t>
         </is>
       </c>
-      <c r="D50" s="4" t="inlineStr">
+      <c r="D50" s="2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E50" s="4" t="inlineStr">
+      <c r="E50" s="2" t="inlineStr">
         <is>
           <t>08/02/2026</t>
         </is>
       </c>
-      <c r="F50" s="4" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G50" s="4" t="inlineStr"/>
-      <c r="H50" s="4" t="inlineStr">
-        <is>
-          <t>0/66</t>
-        </is>
-      </c>
-      <c r="I50" s="4" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F50" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G50" s="2" t="inlineStr"/>
+      <c r="H50" s="2" t="inlineStr">
+        <is>
+          <t>36/66</t>
+        </is>
+      </c>
+      <c r="I50" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-08 12:51:31 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7">
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
@@ -957,7 +957,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>85.3%</t>
+          <t>86.0%</t>
         </is>
       </c>
     </row>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="S15" s="5" t="inlineStr">
         <is>
-          <t>76.0%</t>
+          <t>76.6%</t>
         </is>
       </c>
     </row>
@@ -1373,17 +1373,17 @@
         <v>53</v>
       </c>
       <c r="O16" s="5" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P16" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q16" s="5" t="n">
         <v>4</v>
       </c>
       <c r="R16" s="5" t="inlineStr">
         <is>
-          <t>86.8%</t>
+          <t>88.7%</t>
         </is>
       </c>
       <c r="S16" s="5" t="inlineStr">
@@ -1529,22 +1529,22 @@
         <v>52</v>
       </c>
       <c r="O18" s="5" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P18" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="5" t="n">
         <v>2</v>
       </c>
       <c r="R18" s="5" t="inlineStr">
         <is>
-          <t>94.2%</t>
+          <t>96.2%</t>
         </is>
       </c>
       <c r="S18" s="5" t="inlineStr">
         <is>
-          <t>76.5%</t>
+          <t>75.7%</t>
         </is>
       </c>
     </row>
@@ -3015,7 +3015,7 @@
       <c r="G50" s="2" t="inlineStr"/>
       <c r="H50" s="2" t="inlineStr">
         <is>
-          <t>36/66</t>
+          <t>55/66</t>
         </is>
       </c>
       <c r="I50" s="2" t="inlineStr">
@@ -5046,45 +5046,45 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="4" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B98" s="4" t="inlineStr">
+      <c r="A98" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B98" s="2" t="inlineStr">
         <is>
           <t>B2B</t>
         </is>
       </c>
-      <c r="C98" s="4" t="inlineStr">
+      <c r="C98" s="2" t="inlineStr">
         <is>
           <t>PSYCHIATRY</t>
         </is>
       </c>
-      <c r="D98" s="4" t="inlineStr">
+      <c r="D98" s="2" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="E98" s="4" t="inlineStr">
+      <c r="E98" s="2" t="inlineStr">
         <is>
           <t>08/02/2026</t>
         </is>
       </c>
-      <c r="F98" s="4" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G98" s="4" t="inlineStr"/>
-      <c r="H98" s="4" t="inlineStr">
-        <is>
-          <t>0/62</t>
-        </is>
-      </c>
-      <c r="I98" s="4" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F98" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G98" s="2" t="inlineStr"/>
+      <c r="H98" s="2" t="inlineStr">
+        <is>
+          <t>49/62</t>
+        </is>
+      </c>
+      <c r="I98" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -7802,45 +7802,49 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="4" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B162" s="4" t="inlineStr">
+      <c r="A162" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B162" s="2" t="inlineStr">
         <is>
           <t>B2D</t>
         </is>
       </c>
-      <c r="C162" s="4" t="inlineStr">
+      <c r="C162" s="2" t="inlineStr">
         <is>
           <t>CARDIOLOGY</t>
         </is>
       </c>
-      <c r="D162" s="4" t="inlineStr">
+      <c r="D162" s="2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E162" s="4" t="inlineStr">
+      <c r="E162" s="2" t="inlineStr">
         <is>
           <t>08/02/2026</t>
         </is>
       </c>
-      <c r="F162" s="4" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G162" s="4" t="inlineStr"/>
-      <c r="H162" s="4" t="inlineStr">
-        <is>
-          <t>0/62</t>
-        </is>
-      </c>
-      <c r="I162" s="4" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F162" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G162" s="2" t="inlineStr">
+        <is>
+          <t>fatma_shoukry@hotmail.com</t>
+        </is>
+      </c>
+      <c r="H162" s="2" t="inlineStr">
+        <is>
+          <t>24/62</t>
+        </is>
+      </c>
+      <c r="I162" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-08 18:42:33 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -4818,7 +4818,11 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G92" s="2" t="inlineStr"/>
+      <c r="G92" s="2" t="inlineStr">
+        <is>
+          <t>160534@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H92" s="2" t="inlineStr">
         <is>
           <t>42/62</t>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-09 11:53:31 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7">
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
@@ -957,7 +957,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>86.4%</t>
+          <t>87.2%</t>
         </is>
       </c>
     </row>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>76.0%</t>
+          <t>75.9%</t>
         </is>
       </c>
     </row>
@@ -1295,22 +1295,22 @@
         <v>53</v>
       </c>
       <c r="O15" s="5" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P15" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q15" s="5" t="n">
         <v>3</v>
       </c>
       <c r="R15" s="5" t="inlineStr">
         <is>
-          <t>84.9%</t>
+          <t>86.8%</t>
         </is>
       </c>
       <c r="S15" s="5" t="inlineStr">
         <is>
-          <t>76.6%</t>
+          <t>76.9%</t>
         </is>
       </c>
     </row>
@@ -1451,22 +1451,22 @@
         <v>53</v>
       </c>
       <c r="O17" s="5" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P17" s="5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q17" s="5" t="n">
         <v>5</v>
       </c>
       <c r="R17" s="5" t="inlineStr">
         <is>
-          <t>77.4%</t>
+          <t>79.2%</t>
         </is>
       </c>
       <c r="S17" s="5" t="inlineStr">
         <is>
-          <t>79.2%</t>
+          <t>78.2%</t>
         </is>
       </c>
     </row>
@@ -3033,45 +3033,45 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="4" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B51" s="4" t="inlineStr">
+      <c r="A51" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B51" s="2" t="inlineStr">
         <is>
           <t>B2A</t>
         </is>
       </c>
-      <c r="C51" s="4" t="inlineStr">
+      <c r="C51" s="2" t="inlineStr">
         <is>
           <t>TROPICAL MEDICINE</t>
         </is>
       </c>
-      <c r="D51" s="4" t="inlineStr">
+      <c r="D51" s="2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E51" s="4" t="inlineStr">
+      <c r="E51" s="2" t="inlineStr">
         <is>
           <t>09/02/2026</t>
         </is>
       </c>
-      <c r="F51" s="4" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G51" s="4" t="inlineStr"/>
-      <c r="H51" s="4" t="inlineStr">
-        <is>
-          <t>0/66</t>
-        </is>
-      </c>
-      <c r="I51" s="4" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G51" s="2" t="inlineStr"/>
+      <c r="H51" s="2" t="inlineStr">
+        <is>
+          <t>58/66</t>
+        </is>
+      </c>
+      <c r="I51" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -6993,45 +6993,45 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="4" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B143" s="4" t="inlineStr">
+      <c r="A143" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B143" s="2" t="inlineStr">
         <is>
           <t>B2C</t>
         </is>
       </c>
-      <c r="C143" s="4" t="inlineStr">
+      <c r="C143" s="2" t="inlineStr">
         <is>
           <t>IMMUNOLOGY/HAEMATOLOGY</t>
         </is>
       </c>
-      <c r="D143" s="4" t="inlineStr">
+      <c r="D143" s="2" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="E143" s="4" t="inlineStr">
+      <c r="E143" s="2" t="inlineStr">
         <is>
           <t>09/02/2026</t>
         </is>
       </c>
-      <c r="F143" s="4" t="inlineStr">
+      <c r="F143" s="2" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G143" s="4" t="inlineStr"/>
-      <c r="H143" s="4" t="inlineStr">
-        <is>
-          <t>0/64</t>
-        </is>
-      </c>
-      <c r="I143" s="4" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="G143" s="2" t="inlineStr"/>
+      <c r="H143" s="2" t="inlineStr">
+        <is>
+          <t>24/64</t>
+        </is>
+      </c>
+      <c r="I143" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-09 13:11:59 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7">
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -957,7 +957,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>87.2%</t>
+          <t>87.9%</t>
         </is>
       </c>
     </row>
@@ -1373,17 +1373,17 @@
         <v>53</v>
       </c>
       <c r="O16" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P16" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q16" s="5" t="n">
         <v>3</v>
       </c>
       <c r="R16" s="5" t="inlineStr">
         <is>
-          <t>88.7%</t>
+          <t>90.6%</t>
         </is>
       </c>
       <c r="S16" s="5" t="inlineStr">
@@ -1607,17 +1607,17 @@
         <v>54</v>
       </c>
       <c r="O19" s="5" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P19" s="5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q19" s="5" t="n">
         <v>3</v>
       </c>
       <c r="R19" s="5" t="inlineStr">
         <is>
-          <t>83.3%</t>
+          <t>85.2%</t>
         </is>
       </c>
       <c r="S19" s="5" t="inlineStr">
@@ -5101,45 +5101,45 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="4" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B99" s="4" t="inlineStr">
+      <c r="A99" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B99" s="2" t="inlineStr">
         <is>
           <t>B2B</t>
         </is>
       </c>
-      <c r="C99" s="4" t="inlineStr">
+      <c r="C99" s="2" t="inlineStr">
         <is>
           <t>PSYCHIATRY</t>
         </is>
       </c>
-      <c r="D99" s="4" t="inlineStr">
+      <c r="D99" s="2" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="E99" s="4" t="inlineStr">
+      <c r="E99" s="2" t="inlineStr">
         <is>
           <t>09/02/2026</t>
         </is>
       </c>
-      <c r="F99" s="4" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G99" s="4" t="inlineStr"/>
-      <c r="H99" s="4" t="inlineStr">
-        <is>
-          <t>0/62</t>
-        </is>
-      </c>
-      <c r="I99" s="4" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F99" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G99" s="2" t="inlineStr"/>
+      <c r="H99" s="2" t="inlineStr">
+        <is>
+          <t>48/62</t>
+        </is>
+      </c>
+      <c r="I99" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -10672,45 +10672,45 @@
       </c>
     </row>
     <row r="228">
-      <c r="A228" s="4" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B228" s="4" t="inlineStr">
+      <c r="A228" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B228" s="2" t="inlineStr">
         <is>
           <t>B2E</t>
         </is>
       </c>
-      <c r="C228" s="4" t="inlineStr">
+      <c r="C228" s="2" t="inlineStr">
         <is>
           <t>CHEST</t>
         </is>
       </c>
-      <c r="D228" s="4" t="inlineStr">
+      <c r="D228" s="2" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="E228" s="4" t="inlineStr">
+      <c r="E228" s="2" t="inlineStr">
         <is>
           <t>09/02/2026</t>
         </is>
       </c>
-      <c r="F228" s="4" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G228" s="4" t="inlineStr"/>
-      <c r="H228" s="4" t="inlineStr">
-        <is>
-          <t>0/60</t>
-        </is>
-      </c>
-      <c r="I228" s="4" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F228" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G228" s="2" t="inlineStr"/>
+      <c r="H228" s="2" t="inlineStr">
+        <is>
+          <t>43/60</t>
+        </is>
+      </c>
+      <c r="I228" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-10 07:48:27 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="L8" s="5" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
@@ -1298,10 +1298,10 @@
         <v>46</v>
       </c>
       <c r="P15" s="5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q15" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R15" s="5" t="inlineStr">
         <is>
@@ -1376,10 +1376,10 @@
         <v>48</v>
       </c>
       <c r="P16" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="5" t="n">
         <v>2</v>
-      </c>
-      <c r="Q16" s="5" t="n">
-        <v>3</v>
       </c>
       <c r="R16" s="5" t="inlineStr">
         <is>
@@ -1532,10 +1532,10 @@
         <v>51</v>
       </c>
       <c r="P18" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="5" t="n">
         <v>0</v>
-      </c>
-      <c r="Q18" s="5" t="n">
-        <v>1</v>
       </c>
       <c r="R18" s="5" t="inlineStr">
         <is>
@@ -1610,10 +1610,10 @@
         <v>46</v>
       </c>
       <c r="P19" s="5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q19" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R19" s="5" t="inlineStr">
         <is>
@@ -3076,45 +3076,45 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="9" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B52" s="9" t="inlineStr">
+      <c r="A52" s="4" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B52" s="4" t="inlineStr">
         <is>
           <t>B2A</t>
         </is>
       </c>
-      <c r="C52" s="9" t="inlineStr">
+      <c r="C52" s="4" t="inlineStr">
         <is>
           <t>TROPICAL MEDICINE</t>
         </is>
       </c>
-      <c r="D52" s="9" t="inlineStr">
+      <c r="D52" s="4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E52" s="9" t="inlineStr">
+      <c r="E52" s="4" t="inlineStr">
         <is>
           <t>10/02/2026</t>
         </is>
       </c>
-      <c r="F52" s="9" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G52" s="9" t="inlineStr"/>
-      <c r="H52" s="9" t="inlineStr">
+      <c r="F52" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G52" s="4" t="inlineStr"/>
+      <c r="H52" s="4" t="inlineStr">
         <is>
           <t>0/66</t>
         </is>
       </c>
-      <c r="I52" s="9" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="I52" s="4" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -5144,45 +5144,45 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="9" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B100" s="9" t="inlineStr">
+      <c r="A100" s="4" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B100" s="4" t="inlineStr">
         <is>
           <t>B2B</t>
         </is>
       </c>
-      <c r="C100" s="9" t="inlineStr">
+      <c r="C100" s="4" t="inlineStr">
         <is>
           <t>PSYCHIATRY</t>
         </is>
       </c>
-      <c r="D100" s="9" t="inlineStr">
+      <c r="D100" s="4" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="E100" s="9" t="inlineStr">
+      <c r="E100" s="4" t="inlineStr">
         <is>
           <t>10/02/2026</t>
         </is>
       </c>
-      <c r="F100" s="9" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G100" s="9" t="inlineStr"/>
-      <c r="H100" s="9" t="inlineStr">
+      <c r="F100" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G100" s="4" t="inlineStr"/>
+      <c r="H100" s="4" t="inlineStr">
         <is>
           <t>0/62</t>
         </is>
       </c>
-      <c r="I100" s="9" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="I100" s="4" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -7908,45 +7908,45 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="9" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B164" s="9" t="inlineStr">
+      <c r="A164" s="4" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B164" s="4" t="inlineStr">
         <is>
           <t>B2D</t>
         </is>
       </c>
-      <c r="C164" s="9" t="inlineStr">
+      <c r="C164" s="4" t="inlineStr">
         <is>
           <t>CARDIOLOGY</t>
         </is>
       </c>
-      <c r="D164" s="9" t="inlineStr">
+      <c r="D164" s="4" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E164" s="9" t="inlineStr">
+      <c r="E164" s="4" t="inlineStr">
         <is>
           <t>10/02/2026</t>
         </is>
       </c>
-      <c r="F164" s="9" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G164" s="9" t="inlineStr"/>
-      <c r="H164" s="9" t="inlineStr">
+      <c r="F164" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G164" s="4" t="inlineStr"/>
+      <c r="H164" s="4" t="inlineStr">
         <is>
           <t>0/62</t>
         </is>
       </c>
-      <c r="I164" s="9" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="I164" s="4" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -10715,45 +10715,45 @@
       </c>
     </row>
     <row r="229">
-      <c r="A229" s="9" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B229" s="9" t="inlineStr">
+      <c r="A229" s="4" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B229" s="4" t="inlineStr">
         <is>
           <t>B2E</t>
         </is>
       </c>
-      <c r="C229" s="9" t="inlineStr">
+      <c r="C229" s="4" t="inlineStr">
         <is>
           <t>CHEST</t>
         </is>
       </c>
-      <c r="D229" s="9" t="inlineStr">
+      <c r="D229" s="4" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="E229" s="9" t="inlineStr">
+      <c r="E229" s="4" t="inlineStr">
         <is>
           <t>10/02/2026</t>
         </is>
       </c>
-      <c r="F229" s="9" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G229" s="9" t="inlineStr"/>
-      <c r="H229" s="9" t="inlineStr">
+      <c r="F229" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G229" s="4" t="inlineStr"/>
+      <c r="H229" s="4" t="inlineStr">
         <is>
           <t>0/60</t>
         </is>
       </c>
-      <c r="I229" s="9" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="I229" s="4" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-10 08:57:12 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="L8" s="5" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -1454,10 +1454,10 @@
         <v>42</v>
       </c>
       <c r="P17" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q17" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R17" s="5" t="inlineStr">
         <is>
@@ -7036,45 +7036,45 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="9" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B144" s="9" t="inlineStr">
+      <c r="A144" s="4" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B144" s="4" t="inlineStr">
         <is>
           <t>B2C</t>
         </is>
       </c>
-      <c r="C144" s="9" t="inlineStr">
+      <c r="C144" s="4" t="inlineStr">
         <is>
           <t>IMMUNOLOGY/HAEMATOLOGY</t>
         </is>
       </c>
-      <c r="D144" s="9" t="inlineStr">
+      <c r="D144" s="4" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="E144" s="9" t="inlineStr">
+      <c r="E144" s="4" t="inlineStr">
         <is>
           <t>10/02/2026</t>
         </is>
       </c>
-      <c r="F144" s="9" t="inlineStr">
+      <c r="F144" s="4" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G144" s="9" t="inlineStr"/>
-      <c r="H144" s="9" t="inlineStr">
+      <c r="G144" s="4" t="inlineStr"/>
+      <c r="H144" s="4" t="inlineStr">
         <is>
           <t>0/64</t>
         </is>
       </c>
-      <c r="I144" s="9" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="I144" s="4" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-10 10:09:08 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7">
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
@@ -957,7 +957,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>87.9%</t>
+          <t>88.3%</t>
         </is>
       </c>
     </row>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>75.9%</t>
+          <t>75.7%</t>
         </is>
       </c>
     </row>
@@ -1295,22 +1295,22 @@
         <v>53</v>
       </c>
       <c r="O15" s="5" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P15" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q15" s="5" t="n">
         <v>2</v>
       </c>
       <c r="R15" s="5" t="inlineStr">
         <is>
-          <t>86.8%</t>
+          <t>88.7%</t>
         </is>
       </c>
       <c r="S15" s="5" t="inlineStr">
         <is>
-          <t>76.9%</t>
+          <t>76.1%</t>
         </is>
       </c>
     </row>
@@ -3076,45 +3076,45 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="4" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B52" s="4" t="inlineStr">
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B52" s="2" t="inlineStr">
         <is>
           <t>B2A</t>
         </is>
       </c>
-      <c r="C52" s="4" t="inlineStr">
+      <c r="C52" s="2" t="inlineStr">
         <is>
           <t>TROPICAL MEDICINE</t>
         </is>
       </c>
-      <c r="D52" s="4" t="inlineStr">
+      <c r="D52" s="2" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E52" s="4" t="inlineStr">
+      <c r="E52" s="2" t="inlineStr">
         <is>
           <t>10/02/2026</t>
         </is>
       </c>
-      <c r="F52" s="4" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G52" s="4" t="inlineStr"/>
-      <c r="H52" s="4" t="inlineStr">
-        <is>
-          <t>0/66</t>
-        </is>
-      </c>
-      <c r="I52" s="4" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F52" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G52" s="2" t="inlineStr"/>
+      <c r="H52" s="2" t="inlineStr">
+        <is>
+          <t>27/66</t>
+        </is>
+      </c>
+      <c r="I52" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-10 13:16:21 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7">
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
@@ -957,7 +957,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>88.3%</t>
+          <t>89.1%</t>
         </is>
       </c>
     </row>
@@ -1451,22 +1451,22 @@
         <v>53</v>
       </c>
       <c r="O17" s="5" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P17" s="5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q17" s="5" t="n">
         <v>4</v>
       </c>
       <c r="R17" s="5" t="inlineStr">
         <is>
-          <t>79.2%</t>
+          <t>81.1%</t>
         </is>
       </c>
       <c r="S17" s="5" t="inlineStr">
         <is>
-          <t>78.2%</t>
+          <t>78.0%</t>
         </is>
       </c>
     </row>
@@ -1607,17 +1607,17 @@
         <v>54</v>
       </c>
       <c r="O19" s="5" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P19" s="5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q19" s="5" t="n">
         <v>2</v>
       </c>
       <c r="R19" s="5" t="inlineStr">
         <is>
-          <t>85.2%</t>
+          <t>87.0%</t>
         </is>
       </c>
       <c r="S19" s="5" t="inlineStr">
@@ -6980,10 +6980,14 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G142" s="2" t="inlineStr"/>
+      <c r="G142" s="2" t="inlineStr">
+        <is>
+          <t>160534@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H142" s="2" t="inlineStr">
         <is>
-          <t>13/64</t>
+          <t>36/64</t>
         </is>
       </c>
       <c r="I142" s="2" t="inlineStr">
@@ -7036,45 +7040,45 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="4" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B144" s="4" t="inlineStr">
+      <c r="A144" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B144" s="2" t="inlineStr">
         <is>
           <t>B2C</t>
         </is>
       </c>
-      <c r="C144" s="4" t="inlineStr">
+      <c r="C144" s="2" t="inlineStr">
         <is>
           <t>IMMUNOLOGY/HAEMATOLOGY</t>
         </is>
       </c>
-      <c r="D144" s="4" t="inlineStr">
+      <c r="D144" s="2" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="E144" s="4" t="inlineStr">
+      <c r="E144" s="2" t="inlineStr">
         <is>
           <t>10/02/2026</t>
         </is>
       </c>
-      <c r="F144" s="4" t="inlineStr">
+      <c r="F144" s="2" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G144" s="4" t="inlineStr"/>
-      <c r="H144" s="4" t="inlineStr">
-        <is>
-          <t>0/64</t>
-        </is>
-      </c>
-      <c r="I144" s="4" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="G144" s="2" t="inlineStr"/>
+      <c r="H144" s="2" t="inlineStr">
+        <is>
+          <t>21/64</t>
+        </is>
+      </c>
+      <c r="I144" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -10715,45 +10719,45 @@
       </c>
     </row>
     <row r="229">
-      <c r="A229" s="4" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B229" s="4" t="inlineStr">
+      <c r="A229" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B229" s="2" t="inlineStr">
         <is>
           <t>B2E</t>
         </is>
       </c>
-      <c r="C229" s="4" t="inlineStr">
+      <c r="C229" s="2" t="inlineStr">
         <is>
           <t>CHEST</t>
         </is>
       </c>
-      <c r="D229" s="4" t="inlineStr">
+      <c r="D229" s="2" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="E229" s="4" t="inlineStr">
+      <c r="E229" s="2" t="inlineStr">
         <is>
           <t>10/02/2026</t>
         </is>
       </c>
-      <c r="F229" s="4" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G229" s="4" t="inlineStr"/>
-      <c r="H229" s="4" t="inlineStr">
-        <is>
-          <t>0/60</t>
-        </is>
-      </c>
-      <c r="I229" s="4" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F229" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G229" s="2" t="inlineStr"/>
+      <c r="H229" s="2" t="inlineStr">
+        <is>
+          <t>44/60</t>
+        </is>
+      </c>
+      <c r="I229" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-10 19:11:12 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -1310,7 +1310,7 @@
       </c>
       <c r="S15" s="5" t="inlineStr">
         <is>
-          <t>76.1%</t>
+          <t>76.3%</t>
         </is>
       </c>
     </row>
@@ -3109,7 +3109,7 @@
       <c r="G52" s="2" t="inlineStr"/>
       <c r="H52" s="2" t="inlineStr">
         <is>
-          <t>27/66</t>
+          <t>33/66</t>
         </is>
       </c>
       <c r="I52" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-11 06:50:10 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7">
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="L8" s="5" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
@@ -957,7 +957,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>89.1%</t>
+          <t>89.4%</t>
         </is>
       </c>
     </row>
@@ -1373,22 +1373,22 @@
         <v>53</v>
       </c>
       <c r="O16" s="5" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="P16" s="5" t="n">
         <v>3</v>
       </c>
       <c r="Q16" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R16" s="5" t="inlineStr">
         <is>
-          <t>90.6%</t>
+          <t>92.5%</t>
         </is>
       </c>
       <c r="S16" s="5" t="inlineStr">
         <is>
-          <t>78.1%</t>
+          <t>77.8%</t>
         </is>
       </c>
     </row>
@@ -1454,10 +1454,10 @@
         <v>43</v>
       </c>
       <c r="P17" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q17" s="5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R17" s="5" t="inlineStr">
         <is>
@@ -5187,45 +5187,45 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="9" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B101" s="9" t="inlineStr">
+      <c r="A101" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B101" s="2" t="inlineStr">
         <is>
           <t>B2B</t>
         </is>
       </c>
-      <c r="C101" s="9" t="inlineStr">
+      <c r="C101" s="2" t="inlineStr">
         <is>
           <t>PSYCHIATRY</t>
         </is>
       </c>
-      <c r="D101" s="9" t="inlineStr">
+      <c r="D101" s="2" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="E101" s="9" t="inlineStr">
+      <c r="E101" s="2" t="inlineStr">
         <is>
           <t>11/02/2026</t>
         </is>
       </c>
-      <c r="F101" s="9" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G101" s="9" t="inlineStr"/>
-      <c r="H101" s="9" t="inlineStr">
-        <is>
-          <t>0/62</t>
-        </is>
-      </c>
-      <c r="I101" s="9" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="F101" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G101" s="2" t="inlineStr"/>
+      <c r="H101" s="2" t="inlineStr">
+        <is>
+          <t>40/62</t>
+        </is>
+      </c>
+      <c r="I101" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>
@@ -6434,45 +6434,45 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="9" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B130" s="9" t="inlineStr">
+      <c r="A130" s="4" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B130" s="4" t="inlineStr">
         <is>
           <t>B2C</t>
         </is>
       </c>
-      <c r="C130" s="9" t="inlineStr">
+      <c r="C130" s="4" t="inlineStr">
         <is>
           <t>CLINICAL PATHOLOGY</t>
         </is>
       </c>
-      <c r="D130" s="9" t="inlineStr">
+      <c r="D130" s="4" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E130" s="9" t="inlineStr">
+      <c r="E130" s="4" t="inlineStr">
         <is>
           <t>11/02/2026</t>
         </is>
       </c>
-      <c r="F130" s="9" t="inlineStr">
+      <c r="F130" s="4" t="inlineStr">
         <is>
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G130" s="9" t="inlineStr"/>
-      <c r="H130" s="9" t="inlineStr">
+      <c r="G130" s="4" t="inlineStr"/>
+      <c r="H130" s="4" t="inlineStr">
         <is>
           <t>0/64</t>
         </is>
       </c>
-      <c r="I130" s="9" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="I130" s="4" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-11 08:04:14 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8">
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="L8" s="5" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -1298,10 +1298,10 @@
         <v>47</v>
       </c>
       <c r="P15" s="5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q15" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R15" s="5" t="inlineStr">
         <is>
@@ -1454,10 +1454,10 @@
         <v>43</v>
       </c>
       <c r="P17" s="5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q17" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R17" s="5" t="inlineStr">
         <is>
@@ -1610,10 +1610,10 @@
         <v>47</v>
       </c>
       <c r="P19" s="5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q19" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R19" s="5" t="inlineStr">
         <is>
@@ -3119,45 +3119,45 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="9" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B53" s="9" t="inlineStr">
+      <c r="A53" s="4" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B53" s="4" t="inlineStr">
         <is>
           <t>B2A</t>
         </is>
       </c>
-      <c r="C53" s="9" t="inlineStr">
+      <c r="C53" s="4" t="inlineStr">
         <is>
           <t>TROPICAL MEDICINE</t>
         </is>
       </c>
-      <c r="D53" s="9" t="inlineStr">
+      <c r="D53" s="4" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E53" s="9" t="inlineStr">
+      <c r="E53" s="4" t="inlineStr">
         <is>
           <t>11/02/2026</t>
         </is>
       </c>
-      <c r="F53" s="9" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G53" s="9" t="inlineStr"/>
-      <c r="H53" s="9" t="inlineStr">
+      <c r="F53" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G53" s="4" t="inlineStr"/>
+      <c r="H53" s="4" t="inlineStr">
         <is>
           <t>0/66</t>
         </is>
       </c>
-      <c r="I53" s="9" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="I53" s="4" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -7083,45 +7083,45 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="9" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B145" s="9" t="inlineStr">
+      <c r="A145" s="4" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B145" s="4" t="inlineStr">
         <is>
           <t>B2C</t>
         </is>
       </c>
-      <c r="C145" s="9" t="inlineStr">
+      <c r="C145" s="4" t="inlineStr">
         <is>
           <t>IMMUNOLOGY/HAEMATOLOGY</t>
         </is>
       </c>
-      <c r="D145" s="9" t="inlineStr">
+      <c r="D145" s="4" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="E145" s="9" t="inlineStr">
+      <c r="E145" s="4" t="inlineStr">
         <is>
           <t>11/02/2026</t>
         </is>
       </c>
-      <c r="F145" s="9" t="inlineStr">
+      <c r="F145" s="4" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G145" s="9" t="inlineStr"/>
-      <c r="H145" s="9" t="inlineStr">
+      <c r="G145" s="4" t="inlineStr"/>
+      <c r="H145" s="4" t="inlineStr">
         <is>
           <t>0/64</t>
         </is>
       </c>
-      <c r="I145" s="9" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="I145" s="4" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -10762,45 +10762,45 @@
       </c>
     </row>
     <row r="230">
-      <c r="A230" s="9" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B230" s="9" t="inlineStr">
+      <c r="A230" s="4" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B230" s="4" t="inlineStr">
         <is>
           <t>B2E</t>
         </is>
       </c>
-      <c r="C230" s="9" t="inlineStr">
+      <c r="C230" s="4" t="inlineStr">
         <is>
           <t>CHEST</t>
         </is>
       </c>
-      <c r="D230" s="9" t="inlineStr">
+      <c r="D230" s="4" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="E230" s="9" t="inlineStr">
+      <c r="E230" s="4" t="inlineStr">
         <is>
           <t>11/02/2026</t>
         </is>
       </c>
-      <c r="F230" s="9" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G230" s="9" t="inlineStr"/>
-      <c r="H230" s="9" t="inlineStr">
+      <c r="F230" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G230" s="4" t="inlineStr"/>
+      <c r="H230" s="4" t="inlineStr">
         <is>
           <t>0/60</t>
         </is>
       </c>
-      <c r="I230" s="9" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="I230" s="4" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-11 10:00:44 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7">
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
@@ -957,7 +957,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>89.4%</t>
+          <t>89.8%</t>
         </is>
       </c>
     </row>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>75.7%</t>
+          <t>75.8%</t>
         </is>
       </c>
     </row>
@@ -1295,22 +1295,22 @@
         <v>53</v>
       </c>
       <c r="O15" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P15" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q15" s="5" t="n">
         <v>1</v>
       </c>
       <c r="R15" s="5" t="inlineStr">
         <is>
-          <t>88.7%</t>
+          <t>90.6%</t>
         </is>
       </c>
       <c r="S15" s="5" t="inlineStr">
         <is>
-          <t>76.3%</t>
+          <t>76.6%</t>
         </is>
       </c>
     </row>
@@ -3119,45 +3119,45 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="4" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B53" s="4" t="inlineStr">
+      <c r="A53" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B53" s="2" t="inlineStr">
         <is>
           <t>B2A</t>
         </is>
       </c>
-      <c r="C53" s="4" t="inlineStr">
+      <c r="C53" s="2" t="inlineStr">
         <is>
           <t>TROPICAL MEDICINE</t>
         </is>
       </c>
-      <c r="D53" s="4" t="inlineStr">
+      <c r="D53" s="2" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E53" s="4" t="inlineStr">
+      <c r="E53" s="2" t="inlineStr">
         <is>
           <t>11/02/2026</t>
         </is>
       </c>
-      <c r="F53" s="4" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G53" s="4" t="inlineStr"/>
-      <c r="H53" s="4" t="inlineStr">
-        <is>
-          <t>0/66</t>
-        </is>
-      </c>
-      <c r="I53" s="4" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F53" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G53" s="2" t="inlineStr"/>
+      <c r="H53" s="2" t="inlineStr">
+        <is>
+          <t>60/66</t>
+        </is>
+      </c>
+      <c r="I53" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-11 13:12:08 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7">
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
@@ -957,7 +957,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>89.8%</t>
+          <t>90.2%</t>
         </is>
       </c>
     </row>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>75.8%</t>
+          <t>75.7%</t>
         </is>
       </c>
     </row>
@@ -1607,22 +1607,22 @@
         <v>54</v>
       </c>
       <c r="O19" s="5" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P19" s="5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q19" s="5" t="n">
         <v>1</v>
       </c>
       <c r="R19" s="5" t="inlineStr">
         <is>
-          <t>87.0%</t>
+          <t>88.9%</t>
         </is>
       </c>
       <c r="S19" s="5" t="inlineStr">
         <is>
-          <t>71.5%</t>
+          <t>71.6%</t>
         </is>
       </c>
     </row>
@@ -10762,45 +10762,45 @@
       </c>
     </row>
     <row r="230">
-      <c r="A230" s="4" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B230" s="4" t="inlineStr">
+      <c r="A230" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B230" s="2" t="inlineStr">
         <is>
           <t>B2E</t>
         </is>
       </c>
-      <c r="C230" s="4" t="inlineStr">
+      <c r="C230" s="2" t="inlineStr">
         <is>
           <t>CHEST</t>
         </is>
       </c>
-      <c r="D230" s="4" t="inlineStr">
+      <c r="D230" s="2" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="E230" s="4" t="inlineStr">
+      <c r="E230" s="2" t="inlineStr">
         <is>
           <t>11/02/2026</t>
         </is>
       </c>
-      <c r="F230" s="4" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G230" s="4" t="inlineStr"/>
-      <c r="H230" s="4" t="inlineStr">
-        <is>
-          <t>0/60</t>
-        </is>
-      </c>
-      <c r="I230" s="4" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F230" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G230" s="2" t="inlineStr"/>
+      <c r="H230" s="2" t="inlineStr">
+        <is>
+          <t>44/60</t>
+        </is>
+      </c>
+      <c r="I230" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-11 23:10:07 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -803,7 +803,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7">
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="L8" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -957,7 +957,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>90.2%</t>
+          <t>90.6%</t>
         </is>
       </c>
     </row>
@@ -1373,22 +1373,22 @@
         <v>53</v>
       </c>
       <c r="O16" s="5" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P16" s="5" t="n">
         <v>3</v>
       </c>
       <c r="Q16" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R16" s="5" t="inlineStr">
         <is>
-          <t>92.5%</t>
+          <t>94.3%</t>
         </is>
       </c>
       <c r="S16" s="5" t="inlineStr">
         <is>
-          <t>77.8%</t>
+          <t>77.7%</t>
         </is>
       </c>
     </row>
@@ -5230,45 +5230,45 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="9" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B102" s="9" t="inlineStr">
+      <c r="A102" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B102" s="2" t="inlineStr">
         <is>
           <t>B2B</t>
         </is>
       </c>
-      <c r="C102" s="9" t="inlineStr">
+      <c r="C102" s="2" t="inlineStr">
         <is>
           <t>PSYCHIATRY</t>
         </is>
       </c>
-      <c r="D102" s="9" t="inlineStr">
+      <c r="D102" s="2" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="E102" s="9" t="inlineStr">
+      <c r="E102" s="2" t="inlineStr">
         <is>
           <t>12/02/2026</t>
         </is>
       </c>
-      <c r="F102" s="9" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G102" s="9" t="inlineStr"/>
-      <c r="H102" s="9" t="inlineStr">
-        <is>
-          <t>0/62</t>
-        </is>
-      </c>
-      <c r="I102" s="9" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="F102" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G102" s="2" t="inlineStr"/>
+      <c r="H102" s="2" t="inlineStr">
+        <is>
+          <t>45/62</t>
+        </is>
+      </c>
+      <c r="I102" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-12 07:08:46 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="L8" s="5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -1298,10 +1298,10 @@
         <v>48</v>
       </c>
       <c r="P15" s="5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q15" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15" s="5" t="inlineStr">
         <is>
@@ -1454,10 +1454,10 @@
         <v>43</v>
       </c>
       <c r="P17" s="5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q17" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R17" s="5" t="inlineStr">
         <is>
@@ -1610,10 +1610,10 @@
         <v>48</v>
       </c>
       <c r="P19" s="5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q19" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R19" s="5" t="inlineStr">
         <is>
@@ -3162,45 +3162,45 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="9" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B54" s="9" t="inlineStr">
+      <c r="A54" s="4" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B54" s="4" t="inlineStr">
         <is>
           <t>B2A</t>
         </is>
       </c>
-      <c r="C54" s="9" t="inlineStr">
+      <c r="C54" s="4" t="inlineStr">
         <is>
           <t>TROPICAL MEDICINE</t>
         </is>
       </c>
-      <c r="D54" s="9" t="inlineStr">
+      <c r="D54" s="4" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="E54" s="9" t="inlineStr">
+      <c r="E54" s="4" t="inlineStr">
         <is>
           <t>12/02/2026</t>
         </is>
       </c>
-      <c r="F54" s="9" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G54" s="9" t="inlineStr"/>
-      <c r="H54" s="9" t="inlineStr">
+      <c r="F54" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G54" s="4" t="inlineStr"/>
+      <c r="H54" s="4" t="inlineStr">
         <is>
           <t>0/66</t>
         </is>
       </c>
-      <c r="I54" s="9" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="I54" s="4" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -6477,45 +6477,45 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="9" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B131" s="9" t="inlineStr">
+      <c r="A131" s="4" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B131" s="4" t="inlineStr">
         <is>
           <t>B2C</t>
         </is>
       </c>
-      <c r="C131" s="9" t="inlineStr">
+      <c r="C131" s="4" t="inlineStr">
         <is>
           <t>CLINICAL PATHOLOGY</t>
         </is>
       </c>
-      <c r="D131" s="9" t="inlineStr">
+      <c r="D131" s="4" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="E131" s="9" t="inlineStr">
+      <c r="E131" s="4" t="inlineStr">
         <is>
           <t>12/02/2026</t>
         </is>
       </c>
-      <c r="F131" s="9" t="inlineStr">
+      <c r="F131" s="4" t="inlineStr">
         <is>
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G131" s="9" t="inlineStr"/>
-      <c r="H131" s="9" t="inlineStr">
+      <c r="G131" s="4" t="inlineStr"/>
+      <c r="H131" s="4" t="inlineStr">
         <is>
           <t>0/64</t>
         </is>
       </c>
-      <c r="I131" s="9" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="I131" s="4" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -10805,45 +10805,45 @@
       </c>
     </row>
     <row r="231">
-      <c r="A231" s="9" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B231" s="9" t="inlineStr">
+      <c r="A231" s="4" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B231" s="4" t="inlineStr">
         <is>
           <t>B2E</t>
         </is>
       </c>
-      <c r="C231" s="9" t="inlineStr">
+      <c r="C231" s="4" t="inlineStr">
         <is>
           <t>CHEST</t>
         </is>
       </c>
-      <c r="D231" s="9" t="inlineStr">
+      <c r="D231" s="4" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="E231" s="9" t="inlineStr">
+      <c r="E231" s="4" t="inlineStr">
         <is>
           <t>12/02/2026</t>
         </is>
       </c>
-      <c r="F231" s="9" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G231" s="9" t="inlineStr"/>
-      <c r="H231" s="9" t="inlineStr">
+      <c r="F231" s="4" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G231" s="4" t="inlineStr"/>
+      <c r="H231" s="4" t="inlineStr">
         <is>
           <t>0/60</t>
         </is>
       </c>
-      <c r="I231" s="9" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="I231" s="4" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-12 08:05:03 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -81,7 +81,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -103,9 +103,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -854,7 +851,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -905,7 +902,7 @@
         </is>
       </c>
       <c r="L8" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1454,10 +1451,10 @@
         <v>43</v>
       </c>
       <c r="P17" s="5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q17" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17" s="5" t="inlineStr">
         <is>
@@ -7126,45 +7123,45 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="9" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B146" s="9" t="inlineStr">
+      <c r="A146" s="4" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B146" s="4" t="inlineStr">
         <is>
           <t>B2C</t>
         </is>
       </c>
-      <c r="C146" s="9" t="inlineStr">
+      <c r="C146" s="4" t="inlineStr">
         <is>
           <t>IMMUNOLOGY/HAEMATOLOGY</t>
         </is>
       </c>
-      <c r="D146" s="9" t="inlineStr">
+      <c r="D146" s="4" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="E146" s="9" t="inlineStr">
+      <c r="E146" s="4" t="inlineStr">
         <is>
           <t>12/02/2026</t>
         </is>
       </c>
-      <c r="F146" s="9" t="inlineStr">
+      <c r="F146" s="4" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G146" s="9" t="inlineStr"/>
-      <c r="H146" s="9" t="inlineStr">
+      <c r="G146" s="4" t="inlineStr"/>
+      <c r="H146" s="4" t="inlineStr">
         <is>
           <t>0/64</t>
         </is>
       </c>
-      <c r="I146" s="9" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="I146" s="4" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-12 20:02:14 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -800,7 +800,7 @@
         </is>
       </c>
       <c r="L6" s="5" t="n">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7">
@@ -851,7 +851,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
@@ -954,7 +954,7 @@
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>90.6%</t>
+          <t>90.9%</t>
         </is>
       </c>
     </row>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>75.7%</t>
+          <t>75.8%</t>
         </is>
       </c>
     </row>
@@ -1292,22 +1292,22 @@
         <v>53</v>
       </c>
       <c r="O15" s="5" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="P15" s="5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q15" s="5" t="n">
         <v>0</v>
       </c>
       <c r="R15" s="5" t="inlineStr">
         <is>
-          <t>90.6%</t>
+          <t>92.5%</t>
         </is>
       </c>
       <c r="S15" s="5" t="inlineStr">
         <is>
-          <t>76.6%</t>
+          <t>76.9%</t>
         </is>
       </c>
     </row>
@@ -3159,45 +3159,45 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="4" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B54" s="4" t="inlineStr">
+      <c r="A54" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B54" s="2" t="inlineStr">
         <is>
           <t>B2A</t>
         </is>
       </c>
-      <c r="C54" s="4" t="inlineStr">
+      <c r="C54" s="2" t="inlineStr">
         <is>
           <t>TROPICAL MEDICINE</t>
         </is>
       </c>
-      <c r="D54" s="4" t="inlineStr">
+      <c r="D54" s="2" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="E54" s="4" t="inlineStr">
+      <c r="E54" s="2" t="inlineStr">
         <is>
           <t>12/02/2026</t>
         </is>
       </c>
-      <c r="F54" s="4" t="inlineStr">
-        <is>
-          <t>09:00:00</t>
-        </is>
-      </c>
-      <c r="G54" s="4" t="inlineStr"/>
-      <c r="H54" s="4" t="inlineStr">
-        <is>
-          <t>0/66</t>
-        </is>
-      </c>
-      <c r="I54" s="4" t="inlineStr">
-        <is>
-          <t>Not Recorded</t>
+      <c r="F54" s="2" t="inlineStr">
+        <is>
+          <t>09:00:00</t>
+        </is>
+      </c>
+      <c r="G54" s="2" t="inlineStr"/>
+      <c r="H54" s="2" t="inlineStr">
+        <is>
+          <t>61/66</t>
+        </is>
+      </c>
+      <c r="I54" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-12 21:41:43 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B2_session_analysis.xlsx
@@ -1007,7 +1007,7 @@
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>75.8%</t>
+          <t>75.9%</t>
         </is>
       </c>
     </row>
@@ -1385,7 +1385,7 @@
       </c>
       <c r="S16" s="5" t="inlineStr">
         <is>
-          <t>77.7%</t>
+          <t>78.1%</t>
         </is>
       </c>
     </row>
@@ -5260,7 +5260,7 @@
       <c r="G102" s="2" t="inlineStr"/>
       <c r="H102" s="2" t="inlineStr">
         <is>
-          <t>45/62</t>
+          <t>56/62</t>
         </is>
       </c>
       <c r="I102" s="2" t="inlineStr">

</xml_diff>